<commit_message>
Update environment configuration and Docker setup for vLLM integration. Added vLLM model parameters to .env.example, modified README for vLLM usage instructions, and adjusted Dockerfiles to create non-root users. Updated pipeline results and metadata files for consistency and accuracy.
</commit_message>
<xml_diff>
--- a/pipeline/api/data/results/idea4rc_data_non_repeatable.xlsx
+++ b/pipeline/api/data/results/idea4rc_data_non_repeatable.xlsx
@@ -721,19 +721,11 @@
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>Undifferentiated pleomorphic sarcoma ([8805/3])</t>
-        </is>
-      </c>
+      <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr"/>
       <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>Right thigh</t>
-        </is>
-      </c>
+      <c r="S2" t="inlineStr"/>
       <c r="T2" t="inlineStr"/>
       <c r="U2" t="inlineStr"/>
       <c r="V2" t="inlineStr"/>

</xml_diff>

<commit_message>
Update frontend dependencies and enhance preset management
- Added new dependencies for testing and development, including `@testing-library/jest-dom`, `@testing-library/react`, and `vitest`.
- Updated `package.json` scripts to include testing commands.
- Enhanced `PresetSelector` component to provide feedback messages for loaded presets and warnings for unmatched report types.
- Refactored data loading in `PresetsPage` to improve error handling and loading state management.
- Updated `.gitignore` to include `CLAUDE.md` file.
</commit_message>
<xml_diff>
--- a/pipeline/api/data/results/idea4rc_data_non_repeatable.xlsx
+++ b/pipeline/api/data/results/idea4rc_data_non_repeatable.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AX2"/>
+  <dimension ref="A1:AX3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -686,7 +686,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>TEST001</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -696,48 +696,72 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2023-05-10</t>
+          <t>2023-06-30 10:30:00</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>TEST001</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>58</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr"/>
+          <t>56</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>lorem_ipsum</t>
+        </is>
+      </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2023-06-15</t>
+          <t>2023-06-30 10:30:00</t>
         </is>
       </c>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr"/>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>4298312</t>
+        </is>
+      </c>
       <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr"/>
       <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr"/>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>4090445</t>
+        </is>
+      </c>
       <c r="T2" t="inlineStr"/>
       <c r="U2" t="inlineStr"/>
-      <c r="V2" t="inlineStr"/>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>4228202</t>
+        </is>
+      </c>
       <c r="W2" t="inlineStr"/>
       <c r="X2" t="inlineStr">
         <is>
-          <t>1965</t>
-        </is>
-      </c>
-      <c r="Y2" t="inlineStr"/>
+          <t>1973</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
       <c r="Z2" t="inlineStr"/>
-      <c r="AA2" t="inlineStr"/>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>4329595</t>
+        </is>
+      </c>
       <c r="AB2" t="inlineStr"/>
       <c r="AC2" t="inlineStr"/>
       <c r="AD2" t="inlineStr"/>
@@ -755,16 +779,82 @@
       <c r="AP2" t="inlineStr"/>
       <c r="AQ2" t="inlineStr">
         <is>
-          <t>8507</t>
+          <t>8532</t>
         </is>
       </c>
       <c r="AR2" t="inlineStr"/>
       <c r="AS2" t="inlineStr"/>
-      <c r="AT2" t="inlineStr"/>
-      <c r="AU2" t="inlineStr"/>
-      <c r="AV2" t="inlineStr"/>
+      <c r="AT2" t="inlineStr">
+        <is>
+          <t>2025-04-05 00:00:00</t>
+        </is>
+      </c>
+      <c r="AU2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="AV2" t="inlineStr">
+        <is>
+          <t>2025-04-05 00:00:00</t>
+        </is>
+      </c>
       <c r="AW2" t="inlineStr"/>
       <c r="AX2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr"/>
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr"/>
+      <c r="AB3" t="inlineStr"/>
+      <c r="AC3" t="inlineStr"/>
+      <c r="AD3" t="inlineStr"/>
+      <c r="AE3" t="inlineStr"/>
+      <c r="AF3" t="inlineStr"/>
+      <c r="AG3" t="inlineStr"/>
+      <c r="AH3" t="inlineStr"/>
+      <c r="AI3" t="inlineStr"/>
+      <c r="AJ3" t="inlineStr"/>
+      <c r="AK3" t="inlineStr"/>
+      <c r="AL3" t="inlineStr"/>
+      <c r="AM3" t="inlineStr"/>
+      <c r="AN3" t="inlineStr"/>
+      <c r="AO3" t="inlineStr"/>
+      <c r="AP3" t="inlineStr"/>
+      <c r="AQ3" t="inlineStr"/>
+      <c r="AR3" t="inlineStr"/>
+      <c r="AS3" t="inlineStr"/>
+      <c r="AT3" t="inlineStr"/>
+      <c r="AU3" t="inlineStr"/>
+      <c r="AV3" t="inlineStr"/>
+      <c r="AW3" t="inlineStr"/>
+      <c r="AX3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>